<commit_message>
update Windows Store language info
</commit_message>
<xml_diff>
--- a/StringCodec.UWP/WindowsStore/listingData9N49BK55S2JZ-1152921505688079961.xlsx
+++ b/StringCodec.UWP/WindowsStore/listingData9N49BK55S2JZ-1152921505688079961.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\MS\_projects\vs2017\UWP\StringCodec\StringCodec.UWP\WindowsStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{7F58D8BD-A88F-4FF2-9B31-2E09F54490C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C3428A-EC31-404D-B907-A161D4A313FE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20745" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="listingData9N49BK55S2JZ-1152921" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="286">
   <si>
     <t>Field</t>
   </si>
@@ -52,9 +52,64 @@
     <t>Text</t>
   </si>
   <si>
+    <t># Intro_x000D_
+_x000D_
+This application is text string encode and decode tool._x000D_
+_x000D_
+## Features_x000D_
+_x000D_
+1. URL encode/decode_x000D_
+1. BASE64 encode/decode_x000D_
+1. Raw bytes like \x0d\x0a encode/decode_x000D_
+1. encode small image to base64 string or decode image from base64 string_x000D_
+1. text to QR code, or decode QR code from clipboard image_x000D_
+1. text to some 1D barcode, or decode content from clipboard image_x000D_
+1. rename file or folder name to specified oem charset (UTF8, GBK, BIG5, SHIFT-JIS, ASCII, UNICODE)_x000D_
+1. convert text file content from source charset to target charset (UTF8, GBK, BIG5, SHIFT-JIS, ASCII, UNICODE)</t>
+  </si>
+  <si>
+    <t>これはテキスト文字列のエンコードとデコードのための小さなツールで、結果をクリップボードからクリップボード/ペーストにコピーし、テキストや生成されたイメージを共有することもできます。_x000D_
+_x000D_
+1. URLエンコード/デコード_x000D_
+2. BASE64符号化/復号化_x000D_
+3. 生のバイト、\ x0d \ x0aのような文字列の内容のエンコード/デコード_x000D_
+4. 小さな画像をbase64文字列としてエンコードするか、BASE64文字列から画像をデコードする_x000D_
+5. テキストをQRコードに、またはQR QRコードをクリップボードから_x000D_
+6. いくつかの1Dバーコードへのテキスト、またはクリップボードからのコンテンツのデコード_x000D_
+7. ファイル名またはフォルダ名を指定されたOEM文字セットに変更します（現在、UTF8、GBK、BIG5、SHIFT-JIS、ASCII、UNICODEをサポートしています）_x000D_
+8. ソース・キャラクタ・セットからターゲット・キャラクタ・セットへのテキスト・ファイル・コンテンツの変換（現在はUTF8、GBK、BIG5、SHIFT-JIS、ASCII、UNICODEをサポートしています）</t>
+  </si>
+  <si>
+    <t>这是一个用于文本字符串编码和解码小工具, 可以复制结果到剪贴板/从剪贴板粘贴以及共享文本或生成的图片._x000D_
+_x000D_
+1. URL编码/解码_x000D_
+2. BASE64编码/解码_x000D_
+3. 原始字节，如\x0d\x0a这样的字符串内容的编码/解码_x000D_
+4. 将小图像编码为base64字符串或从BASE64 字符串解码图像_x000D_
+5. 文本到QR码，或从剪贴板图像解码QR二维码_x000D_
+6. 文本到一些一维条形码，或从剪贴板图像解码内容_x000D_
+7. 将文件或文件夹名称重命名为指定的 OEM 字符集（现支持 UTF8，GBK，BIG5，SHIFT-JIS，ASCII，UNICODE）_x000D_
+8. 将文本文件内容从源字符集转换为目标字符集（现支持 UTF8，GBK，BIG5，SHIFT-JIS，ASCII，UNICODE）</t>
+  </si>
+  <si>
+    <t>這是一個用於文本字符串編碼和解碼小工具。備註: 截圖和簡體中文沒什麼區別, 就不重複上傳了._x000D_
+_x000D_
+1. URL編碼/解碼_x000D_
+2. BASE64編碼/解碼_x000D_
+3. 原始字節，如\x0d\x0a這樣的字符串內容的編碼/解碼_x000D_
+4. 將小圖像編碼為base64字符串或從BASE64 字符串解碼圖像_x000D_
+5. 文本到QR碼，或從剪貼板圖像解碼QR二維碼_x000D_
+6. 文本到一些一維條形碼，或從剪貼板圖像解碼內容_x000D_
+7. 將檔案或檔案夾名稱重命名為指定的 OEM 字符集（現支持 UTF8，GBK，BIG5，SHIFT-JIS，ASCII，UNICODE）_x000D_
+8. 將文本檔案內容從源字符集轉換為目標字符集（現支持 UTF8，GBK，BIG5，SHIFT-JIS，ASCII，UNICODE）</t>
+  </si>
+  <si>
     <t>ReleaseNotes</t>
   </si>
   <si>
+    <t>表示される日本語のテキストのほとんどはMicrosoft機械翻訳によるものですので、ご迷惑をおかけしてください。</t>
+  </si>
+  <si>
     <t>Title</t>
   </si>
   <si>
@@ -97,63 +152,243 @@
     <t>Relative path (or URL to file in Dev Center)</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017839999</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845202</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843766</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118348/listingassets/2000000000017843164</t>
+  </si>
+  <si>
     <t>DesktopScreenshot2</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840226</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845207</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843910</t>
+  </si>
+  <si>
     <t>DesktopScreenshot3</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840292</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845261</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843911</t>
+  </si>
+  <si>
     <t>DesktopScreenshot4</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840297</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845263</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843912</t>
+  </si>
+  <si>
     <t>DesktopScreenshot5</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840347</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845268</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843913</t>
+  </si>
+  <si>
     <t>DesktopScreenshot6</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840421</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845306</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843915</t>
+  </si>
+  <si>
     <t>DesktopScreenshot7</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840425</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845323</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843916</t>
+  </si>
+  <si>
     <t>DesktopScreenshot8</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840535</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845367</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017843919</t>
+  </si>
+  <si>
     <t>DesktopScreenshot9</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840582</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845396</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017844091</t>
+  </si>
+  <si>
     <t>DesktopScreenshot10</t>
   </si>
   <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118342/listingassets/2000000000017840588</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118344/listingassets/2000000000017845414</t>
+  </si>
+  <si>
+    <t>https://developer.microsoft.com/en-us/dashboard/apps/9N49BK55S2JZ/submissions/1152921505688079961/listings/1152922700001118346/listingassets/2000000000017844095</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption1</t>
   </si>
   <si>
+    <t>Main UI</t>
+  </si>
+  <si>
+    <t>テキストコーデック表示</t>
+  </si>
+  <si>
+    <t>导航视图</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption2</t>
   </si>
   <si>
+    <t>QR Encode and Decode UI</t>
+  </si>
+  <si>
+    <t>ナビゲーションビュー</t>
+  </si>
+  <si>
+    <t>文本编码解码视图</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption3</t>
   </si>
   <si>
+    <t>Small Image From/To BASE64 UI</t>
+  </si>
+  <si>
+    <t>QRコード生成/解釈ビュー</t>
+  </si>
+  <si>
+    <t>二维码生成/解读视图</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption4</t>
   </si>
   <si>
+    <t>Common 1-D Barcode Encode and Decode UI</t>
+  </si>
+  <si>
+    <t>BASE64と画像変換ビュー</t>
+  </si>
+  <si>
+    <t>一维条码生成/解码视图</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption5</t>
   </si>
   <si>
+    <t>QR Code and 1D Barcode Foreground/Background Color picker dialog</t>
+  </si>
+  <si>
+    <t>バーコード生成/復号化ビュー</t>
+  </si>
+  <si>
+    <t>二维码/条码颜色选取对话框</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption6</t>
   </si>
   <si>
+    <t>Common QR Code Builder UI</t>
+  </si>
+  <si>
+    <t>特定のコンテンツのQRコード生成ビュー</t>
+  </si>
+  <si>
+    <t>特定内容的二维码生成视图</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption7</t>
   </si>
   <si>
+    <t>Common QR Code options flyout</t>
+  </si>
+  <si>
+    <t>指定したファイル/フォルダを開き、ファイル/フォルダ名を指定した文字セットに変更するか、ソースファイルセットから指定した文字セットに変更します</t>
+  </si>
+  <si>
+    <t>打开指定的文件/文件夹, 以便对文件/文件夹的名称做指定字符集的重命名或者文本文件的内容从源字符集转换为指定的字符集</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption8</t>
   </si>
   <si>
+    <t>File and Folder rename/convert UI with source Shift-JIS text</t>
+  </si>
+  <si>
+    <t>上のコマンドボタンバーで、名前の変更/変換ボタンを右クリックして、関連するオプションを表示します。</t>
+  </si>
+  <si>
+    <t>选中一个文件或者文件后, 就可以右键弹出快捷菜单以便重命名/文本内容转换</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption9</t>
   </si>
   <si>
+    <t>when selected one item you can right-click mouse/right tapped to popup a context flyout for fast rename/convert item</t>
+  </si>
+  <si>
+    <t>在上方的命令按钮条上, 右键点击重命名/转换按钮会弹出相关的选项.</t>
+  </si>
+  <si>
     <t>DesktopScreenshotCaption10</t>
   </si>
   <si>
+    <t>right-click or right tapped on rename/convert AppBar command button, will popup the options for rename/convert</t>
+  </si>
+  <si>
+    <t>ビューセット、あなたが今、窓ダーク/ライトのテーマだけでなく、ユーザーインターフェースの言語を設定することができます流暢ではないが、私を許してください場合は、今、機械翻訳のための英語/簡体字中国語/繁体字中国語/日本語、日本語ベースのインターフェイスをサポートしています</t>
+  </si>
+  <si>
+    <t>设定视图, 现在可以设定窗口主题深色/浅色, 以及用户界面的语言, 现在支持英语/简体中文/繁体中文/日语, 日语界面为机器翻译为主, 如有不通顺请见谅</t>
+  </si>
+  <si>
     <t>MobileScreenshot1</t>
   </si>
   <si>
@@ -382,12 +617,33 @@
     <t>Feature1</t>
   </si>
   <si>
+    <t>Text From/To URL, BASE64, QRCODE, BARCODE...</t>
+  </si>
+  <si>
+    <t>BASE64コーデック画像</t>
+  </si>
+  <si>
+    <t>BASE64 编解码图像</t>
+  </si>
+  <si>
     <t>Feature2</t>
   </si>
   <si>
+    <t>QRコードQRコードを生成する</t>
+  </si>
+  <si>
+    <t>生成QRCode二维码</t>
+  </si>
+  <si>
     <t>Feature3</t>
   </si>
   <si>
+    <t>テキストまたはQRコード/画像を共有する</t>
+  </si>
+  <si>
+    <t>共享文本或者二维码/图像</t>
+  </si>
+  <si>
     <t>Feature4</t>
   </si>
   <si>
@@ -662,19 +918,6 @@
   </si>
   <si>
     <t>TrailerThumbnail15</t>
-  </si>
-  <si>
-    <t>This application is text string encode and decode tool.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>此应用程序是文本字符串编码和解码工具。</t>
-  </si>
-  <si>
-    <t>此程式是文本字符串編碼和解碼工具。</t>
-  </si>
-  <si>
-    <t>このプログラムは、テキスト文字列のエンコードとデコードのツールです。</t>
   </si>
 </sst>
 </file>
@@ -1267,9 +1510,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1628,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1637,10 +1883,11 @@
     <col min="1" max="1" width="30.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.125" customWidth="1"/>
-    <col min="7" max="7" width="35.5" customWidth="1"/>
-    <col min="8" max="8" width="36.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.25" customWidth="1"/>
+    <col min="6" max="6" width="46.125" customWidth="1"/>
+    <col min="7" max="7" width="41.625" customWidth="1"/>
+    <col min="8" max="8" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1669,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="313.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1679,22 +1926,22 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H2" t="s">
-        <v>216</v>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1702,10 +1949,13 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1713,25 +1963,22 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1739,13 +1986,10 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1756,7 +2000,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1767,7 +2011,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -1778,7 +2022,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -1789,7 +2033,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -1800,7 +2044,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -1811,117 +2055,210 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B21">
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <v>150</v>
@@ -1929,10 +2266,19 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>151</v>
@@ -1940,10 +2286,19 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B24">
         <v>152</v>
@@ -1951,10 +2306,19 @@
       <c r="C24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>153</v>
@@ -1962,10 +2326,19 @@
       <c r="C25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="B26">
         <v>154</v>
@@ -1973,10 +2346,19 @@
       <c r="C26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B27">
         <v>155</v>
@@ -1984,10 +2366,19 @@
       <c r="C27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="B28">
         <v>156</v>
@@ -1995,10 +2386,19 @@
       <c r="C28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B29">
         <v>157</v>
@@ -2006,10 +2406,19 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="B30">
         <v>158</v>
@@ -2017,10 +2426,19 @@
       <c r="C30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="B31">
         <v>159</v>
@@ -2028,120 +2446,129 @@
       <c r="C31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="B33">
         <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B34">
         <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="B35">
         <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="B36">
         <v>204</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="B37">
         <v>205</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="B38">
         <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="B39">
         <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="B40">
         <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B41">
         <v>209</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B42">
         <v>250</v>
@@ -2152,7 +2579,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="B43">
         <v>251</v>
@@ -2163,7 +2590,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="B44">
         <v>252</v>
@@ -2174,7 +2601,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="B45">
         <v>253</v>
@@ -2185,7 +2612,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="B46">
         <v>254</v>
@@ -2196,7 +2623,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B47">
         <v>255</v>
@@ -2207,7 +2634,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="B48">
         <v>256</v>
@@ -2218,7 +2645,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B49">
         <v>257</v>
@@ -2229,7 +2656,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B50">
         <v>258</v>
@@ -2240,7 +2667,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="B51">
         <v>259</v>
@@ -2251,117 +2678,117 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B52">
         <v>300</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B53">
         <v>301</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="B54">
         <v>302</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B55">
         <v>303</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="B56">
         <v>304</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="B57">
         <v>305</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="B58">
         <v>306</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="B59">
         <v>307</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="B60">
         <v>308</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="B61">
         <v>309</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="B62">
         <v>350</v>
@@ -2372,7 +2799,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="B63">
         <v>351</v>
@@ -2383,7 +2810,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="B64">
         <v>352</v>
@@ -2394,7 +2821,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="B65">
         <v>353</v>
@@ -2405,7 +2832,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="B66">
         <v>354</v>
@@ -2416,7 +2843,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="B67">
         <v>355</v>
@@ -2427,7 +2854,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="B68">
         <v>356</v>
@@ -2438,7 +2865,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="B69">
         <v>357</v>
@@ -2449,7 +2876,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="B70">
         <v>358</v>
@@ -2460,7 +2887,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="B71">
         <v>359</v>
@@ -2471,117 +2898,117 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="B72">
         <v>400</v>
       </c>
       <c r="C72" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="B73">
         <v>401</v>
       </c>
       <c r="C73" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="B74">
         <v>402</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="B75">
         <v>403</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="B76">
         <v>404</v>
       </c>
       <c r="C76" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="B77">
         <v>405</v>
       </c>
       <c r="C77" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="B78">
         <v>406</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="B79">
         <v>407</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>157</v>
       </c>
       <c r="B80">
         <v>408</v>
       </c>
       <c r="C80" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="B81">
         <v>409</v>
       </c>
       <c r="C81" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="B82">
         <v>450</v>
@@ -2592,7 +3019,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="B83">
         <v>451</v>
@@ -2603,7 +3030,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B84">
         <v>452</v>
@@ -2614,7 +3041,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="B85">
         <v>453</v>
@@ -2625,7 +3052,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="B86">
         <v>454</v>
@@ -2636,7 +3063,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="B87">
         <v>455</v>
@@ -2647,7 +3074,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="B88">
         <v>456</v>
@@ -2658,7 +3085,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="B89">
         <v>457</v>
@@ -2669,7 +3096,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="B90">
         <v>458</v>
@@ -2680,7 +3107,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B91">
         <v>459</v>
@@ -2691,46 +3118,46 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
       <c r="B92">
         <v>600</v>
       </c>
       <c r="C92" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="B93">
         <v>601</v>
       </c>
       <c r="C93" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="B94">
         <v>602</v>
       </c>
       <c r="C94" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="B95">
         <v>603</v>
       </c>
       <c r="C95" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -2747,117 +3174,117 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
       <c r="B96">
         <v>604</v>
       </c>
       <c r="C96" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="B97">
         <v>605</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
       <c r="B98">
         <v>606</v>
       </c>
       <c r="C98" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="B99">
         <v>607</v>
       </c>
       <c r="C99" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="B100">
         <v>608</v>
       </c>
       <c r="C100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="B101">
         <v>609</v>
       </c>
       <c r="C101" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="B102">
         <v>610</v>
       </c>
       <c r="C102" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="B103">
         <v>611</v>
       </c>
       <c r="C103" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>182</v>
       </c>
       <c r="B104">
         <v>612</v>
       </c>
       <c r="C104" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>183</v>
       </c>
       <c r="B105">
         <v>613</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="B106">
         <v>700</v>
@@ -2865,10 +3292,22 @@
       <c r="C106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E106" t="s">
+        <v>185</v>
+      </c>
+      <c r="F106" t="s">
+        <v>186</v>
+      </c>
+      <c r="G106" t="s">
+        <v>187</v>
+      </c>
+      <c r="H106" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="B107">
         <v>701</v>
@@ -2876,10 +3315,19 @@
       <c r="C107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F107" t="s">
+        <v>189</v>
+      </c>
+      <c r="G107" t="s">
+        <v>190</v>
+      </c>
+      <c r="H107" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="B108">
         <v>702</v>
@@ -2887,10 +3335,19 @@
       <c r="C108" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>192</v>
+      </c>
+      <c r="G108" t="s">
+        <v>193</v>
+      </c>
+      <c r="H108" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>194</v>
       </c>
       <c r="B109">
         <v>703</v>
@@ -2899,9 +3356,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="B110">
         <v>704</v>
@@ -2910,9 +3367,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="B111">
         <v>705</v>
@@ -2921,9 +3378,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="B112">
         <v>706</v>
@@ -2934,7 +3391,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>198</v>
       </c>
       <c r="B113">
         <v>707</v>
@@ -2945,7 +3402,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="B114">
         <v>708</v>
@@ -2956,7 +3413,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>200</v>
       </c>
       <c r="B115">
         <v>709</v>
@@ -2967,7 +3424,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>201</v>
       </c>
       <c r="B116">
         <v>710</v>
@@ -2978,7 +3435,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B117">
         <v>711</v>
@@ -2989,7 +3446,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
       <c r="B118">
         <v>712</v>
@@ -3000,7 +3457,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="B119">
         <v>713</v>
@@ -3011,7 +3468,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="B120">
         <v>714</v>
@@ -3022,7 +3479,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="B121">
         <v>715</v>
@@ -3033,7 +3490,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="B122">
         <v>716</v>
@@ -3044,7 +3501,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>208</v>
       </c>
       <c r="B123">
         <v>717</v>
@@ -3055,7 +3512,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="B124">
         <v>718</v>
@@ -3066,7 +3523,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
       <c r="B125">
         <v>719</v>
@@ -3077,7 +3534,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="B126">
         <v>800</v>
@@ -3088,7 +3545,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="B127">
         <v>801</v>
@@ -3099,7 +3556,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
       <c r="B128">
         <v>802</v>
@@ -3110,7 +3567,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="B129">
         <v>803</v>
@@ -3121,7 +3578,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
       <c r="B130">
         <v>804</v>
@@ -3132,7 +3589,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>144</v>
+        <v>216</v>
       </c>
       <c r="B131">
         <v>805</v>
@@ -3143,7 +3600,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="B132">
         <v>806</v>
@@ -3154,7 +3611,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="B133">
         <v>807</v>
@@ -3165,7 +3622,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="B134">
         <v>808</v>
@@ -3176,7 +3633,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="B135">
         <v>809</v>
@@ -3187,7 +3644,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="B136">
         <v>810</v>
@@ -3198,7 +3655,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>150</v>
+        <v>222</v>
       </c>
       <c r="B137">
         <v>850</v>
@@ -3209,7 +3666,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="B138">
         <v>851</v>
@@ -3220,7 +3677,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>224</v>
       </c>
       <c r="B139">
         <v>852</v>
@@ -3231,7 +3688,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="B140">
         <v>853</v>
@@ -3242,7 +3699,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>154</v>
+        <v>226</v>
       </c>
       <c r="B141">
         <v>854</v>
@@ -3253,7 +3710,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="B142">
         <v>855</v>
@@ -3264,7 +3721,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="B143">
         <v>856</v>
@@ -3275,7 +3732,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="B144">
         <v>857</v>
@@ -3286,7 +3743,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="B145">
         <v>858</v>
@@ -3297,7 +3754,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>159</v>
+        <v>231</v>
       </c>
       <c r="B146">
         <v>859</v>
@@ -3308,7 +3765,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="B147">
         <v>860</v>
@@ -3319,7 +3776,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>233</v>
       </c>
       <c r="B148">
         <v>900</v>
@@ -3330,7 +3787,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>234</v>
       </c>
       <c r="B149">
         <v>901</v>
@@ -3341,7 +3798,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>235</v>
       </c>
       <c r="B150">
         <v>902</v>
@@ -3352,7 +3809,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="B151">
         <v>903</v>
@@ -3363,7 +3820,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="B152">
         <v>904</v>
@@ -3374,7 +3831,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>166</v>
+        <v>238</v>
       </c>
       <c r="B153">
         <v>905</v>
@@ -3385,7 +3842,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>167</v>
+        <v>239</v>
       </c>
       <c r="B154">
         <v>906</v>
@@ -3396,183 +3853,183 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>168</v>
+        <v>240</v>
       </c>
       <c r="B155">
         <v>999</v>
       </c>
       <c r="C155" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
       <c r="B156">
         <v>1000</v>
       </c>
       <c r="C156" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>170</v>
+        <v>242</v>
       </c>
       <c r="B157">
         <v>1001</v>
       </c>
       <c r="C157" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>171</v>
+        <v>243</v>
       </c>
       <c r="B158">
         <v>1002</v>
       </c>
       <c r="C158" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>172</v>
+        <v>244</v>
       </c>
       <c r="B159">
         <v>1003</v>
       </c>
       <c r="C159" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>173</v>
+        <v>245</v>
       </c>
       <c r="B160">
         <v>1004</v>
       </c>
       <c r="C160" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>174</v>
+        <v>246</v>
       </c>
       <c r="B161">
         <v>1005</v>
       </c>
       <c r="C161" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>175</v>
+        <v>247</v>
       </c>
       <c r="B162">
         <v>1006</v>
       </c>
       <c r="C162" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>176</v>
+        <v>248</v>
       </c>
       <c r="B163">
         <v>1007</v>
       </c>
       <c r="C163" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>177</v>
+        <v>249</v>
       </c>
       <c r="B164">
         <v>1008</v>
       </c>
       <c r="C164" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>178</v>
+        <v>250</v>
       </c>
       <c r="B165">
         <v>1009</v>
       </c>
       <c r="C165" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="B166">
         <v>1010</v>
       </c>
       <c r="C166" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>180</v>
+        <v>252</v>
       </c>
       <c r="B167">
         <v>1011</v>
       </c>
       <c r="C167" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>181</v>
+        <v>253</v>
       </c>
       <c r="B168">
         <v>1012</v>
       </c>
       <c r="C168" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>182</v>
+        <v>254</v>
       </c>
       <c r="B169">
         <v>1013</v>
       </c>
       <c r="C169" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="B170">
         <v>1014</v>
       </c>
       <c r="C170" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>184</v>
+        <v>256</v>
       </c>
       <c r="B171">
         <v>1020</v>
@@ -3583,7 +4040,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="B172">
         <v>1021</v>
@@ -3594,7 +4051,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>186</v>
+        <v>258</v>
       </c>
       <c r="B173">
         <v>1022</v>
@@ -3605,7 +4062,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>187</v>
+        <v>259</v>
       </c>
       <c r="B174">
         <v>1023</v>
@@ -3616,7 +4073,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
       <c r="B175">
         <v>1024</v>
@@ -3627,7 +4084,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
       <c r="B176">
         <v>1025</v>
@@ -3638,7 +4095,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="B177">
         <v>1026</v>
@@ -3649,7 +4106,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>191</v>
+        <v>263</v>
       </c>
       <c r="B178">
         <v>1027</v>
@@ -3660,7 +4117,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>192</v>
+        <v>264</v>
       </c>
       <c r="B179">
         <v>1028</v>
@@ -3671,7 +4128,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>193</v>
+        <v>265</v>
       </c>
       <c r="B180">
         <v>1029</v>
@@ -3682,7 +4139,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>194</v>
+        <v>266</v>
       </c>
       <c r="B181">
         <v>1030</v>
@@ -3693,7 +4150,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>195</v>
+        <v>267</v>
       </c>
       <c r="B182">
         <v>1031</v>
@@ -3704,7 +4161,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="B183">
         <v>1032</v>
@@ -3715,7 +4172,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="B184">
         <v>1033</v>
@@ -3726,7 +4183,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>198</v>
+        <v>270</v>
       </c>
       <c r="B185">
         <v>1034</v>
@@ -3737,172 +4194,171 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>199</v>
+        <v>271</v>
       </c>
       <c r="B186">
         <v>1040</v>
       </c>
       <c r="C186" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>200</v>
+        <v>272</v>
       </c>
       <c r="B187">
         <v>1041</v>
       </c>
       <c r="C187" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>201</v>
+        <v>273</v>
       </c>
       <c r="B188">
         <v>1042</v>
       </c>
       <c r="C188" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="B189">
         <v>1043</v>
       </c>
       <c r="C189" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>203</v>
+        <v>275</v>
       </c>
       <c r="B190">
         <v>1044</v>
       </c>
       <c r="C190" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>204</v>
+        <v>276</v>
       </c>
       <c r="B191">
         <v>1045</v>
       </c>
       <c r="C191" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>205</v>
+        <v>277</v>
       </c>
       <c r="B192">
         <v>1046</v>
       </c>
       <c r="C192" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="B193">
         <v>1047</v>
       </c>
       <c r="C193" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="B194">
         <v>1048</v>
       </c>
       <c r="C194" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
       <c r="B195">
         <v>1049</v>
       </c>
       <c r="C195" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
       <c r="B196">
         <v>1050</v>
       </c>
       <c r="C196" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>210</v>
+        <v>282</v>
       </c>
       <c r="B197">
         <v>1051</v>
       </c>
       <c r="C197" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>211</v>
+        <v>283</v>
       </c>
       <c r="B198">
         <v>1052</v>
       </c>
       <c r="C198" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="B199">
         <v>1053</v>
       </c>
       <c r="C199" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>213</v>
+        <v>285</v>
       </c>
       <c r="B200">
         <v>1054</v>
       </c>
       <c r="C200" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>